<commit_message>
Addition of test xml for jenkins
</commit_message>
<xml_diff>
--- a/binaries/FCfiles/ManageProducts.xlsx
+++ b/binaries/FCfiles/ManageProducts.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
   <si>
     <t>Other</t>
   </si>
@@ -160,6 +160,18 @@
   </si>
   <si>
     <t>prodtYHO</t>
+  </si>
+  <si>
+    <t>produOai</t>
+  </si>
+  <si>
+    <t>prodzqOe</t>
+  </si>
+  <si>
+    <t>prodLxOo</t>
+  </si>
+  <si>
+    <t>prodrHEk</t>
   </si>
 </sst>
 </file>
@@ -182,7 +194,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="41">
+  <fills count="49">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -384,8 +396,48 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="40">
+  <borders count="48">
     <border>
       <left/>
       <right/>
@@ -586,11 +638,39 @@
       <top style="thin"/>
       <bottom style="thin"/>
     </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="1" applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
@@ -618,7 +698,11 @@
     <xf applyBorder="true" applyFill="true" borderId="33" fillId="34" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="35" fillId="36" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyBorder="true" applyFill="true" borderId="37" fillId="38" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="39" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="true" applyFill="true" borderId="39" fillId="40" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="41" fillId="42" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="43" fillId="44" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="45" fillId="46" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="48" borderId="47" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle builtinId="0" name="Normal" xfId="0"/>
@@ -968,8 +1052,8 @@
       <c r="A2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="12" t="s">
-        <v>29</v>
+      <c r="B2" s="28" t="s">
+        <v>45</v>
       </c>
       <c r="C2" s="9" t="s">
         <v>23</v>
@@ -1049,8 +1133,8 @@
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="13" t="s">
-        <v>30</v>
+      <c r="B5" s="29" t="s">
+        <v>46</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>23</v>
@@ -1139,8 +1223,8 @@
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="27" t="s">
-        <v>44</v>
+      <c r="B8" s="31" t="s">
+        <v>48</v>
       </c>
       <c r="C8" s="9" t="s">
         <v>22</v>

</xml_diff>